<commit_message>
Commit after jenkins integration
</commit_message>
<xml_diff>
--- a/Resources/Exceldriven.xlsx
+++ b/Resources/Exceldriven.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikatkar\girrepo\git-sample-repo\testng_Realtime\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikatkar\git\testng_Realtime\testng_Realtime\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990B1467-3EC5-4C75-9D0F-4D8CFFC6DD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF5812-B46B-459E-ADB0-578D2079CD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>Verifyloginout</t>
-  </si>
-  <si>
     <t>kirankatkar3317@gmail.com</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>Kiran@3318</t>
+  </si>
+  <si>
+    <t>Verifyloginoutwithalltests</t>
   </si>
 </sst>
 </file>
@@ -366,42 +366,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE1019B-C8E6-4AC3-A0AB-D4ED6F422DDC}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>